<commit_message>
arrumando o problema do Marcus
</commit_message>
<xml_diff>
--- a/Forms/Form_161.xlsx
+++ b/Forms/Form_161.xlsx
@@ -792,8 +792,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="###\-####"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="0_ ;\-0\ "/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1768,56 +1768,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1831,71 +1823,15 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1932,10 +1868,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1950,6 +1882,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1959,51 +1897,203 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2011,98 +2101,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2142,7 +2142,7 @@
         <xdr:cNvPr id="2" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6EE015BE-D3BC-413F-A204-C9E16EA19145}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EE015BE-D3BC-413F-A204-C9E16EA19145}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2203,7 +2203,7 @@
         <xdr:cNvPr id="3" name="Retângulo 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A9EC258-2B9E-48CA-8307-7D25F3FF3ED0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A9EC258-2B9E-48CA-8307-7D25F3FF3ED0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2269,7 +2269,7 @@
         <xdr:cNvPr id="4" name="Retângulo 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EB284875-99DB-4748-A778-0E92ECC762DD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB284875-99DB-4748-A778-0E92ECC762DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2330,7 +2330,7 @@
         <xdr:cNvPr id="6" name="CaixaDeTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00FCFFFA-FF5D-4FF4-81E5-906E2CC1ACC1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00FCFFFA-FF5D-4FF4-81E5-906E2CC1ACC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2388,7 +2388,7 @@
         <xdr:cNvPr id="7" name="CaixaDeTexto 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29EE3EC1-C544-4AA9-9D64-FB8A722D38A4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29EE3EC1-C544-4AA9-9D64-FB8A722D38A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2459,7 +2459,7 @@
         <xdr:cNvPr id="8" name="Retângulo 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ACA2AA39-5C5C-48C8-8ED0-46677B85F7A7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACA2AA39-5C5C-48C8-8ED0-46677B85F7A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2525,7 +2525,7 @@
         <xdr:cNvPr id="9" name="Retângulo 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E149FAD1-A4B7-4D6B-8BC0-DB1D7F8454ED}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E149FAD1-A4B7-4D6B-8BC0-DB1D7F8454ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2591,7 +2591,7 @@
         <xdr:cNvPr id="48" name="Retângulo 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C3E30EE1-BB65-4BE3-9605-3B1B2E596710}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3E30EE1-BB65-4BE3-9605-3B1B2E596710}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2652,7 +2652,7 @@
         <xdr:cNvPr id="49" name="CaixaDeTexto 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B3177E40-44A7-4EAA-86FD-DB148E89C3E0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3177E40-44A7-4EAA-86FD-DB148E89C3E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2710,7 +2710,7 @@
         <xdr:cNvPr id="50" name="CaixaDeTexto 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61CC7ED0-9ECE-4FE3-BF1D-8C3096D2A4BD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61CC7ED0-9ECE-4FE3-BF1D-8C3096D2A4BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2781,7 +2781,7 @@
         <xdr:cNvPr id="51" name="Retângulo 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{81235F38-066B-4877-8D81-1B42440FD6BF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81235F38-066B-4877-8D81-1B42440FD6BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2847,7 +2847,7 @@
         <xdr:cNvPr id="52" name="Retângulo 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66327A3A-DB18-420E-8B4A-6F1EB64889AD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66327A3A-DB18-420E-8B4A-6F1EB64889AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2908,7 +2908,7 @@
         <xdr:cNvPr id="53" name="CaixaDeTexto 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5A348048-9BEB-4E5B-BCE8-1E8AC20C4B14}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A348048-9BEB-4E5B-BCE8-1E8AC20C4B14}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2966,7 +2966,7 @@
         <xdr:cNvPr id="54" name="CaixaDeTexto 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61E3086A-B31C-4B44-B6A5-467027A1CA1C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61E3086A-B31C-4B44-B6A5-467027A1CA1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3037,7 +3037,7 @@
         <xdr:cNvPr id="55" name="Retângulo 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F4243475-2C9D-48EB-B608-2C206C9E8E14}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4243475-2C9D-48EB-B608-2C206C9E8E14}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3103,7 +3103,7 @@
         <xdr:cNvPr id="56" name="Retângulo 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{19A48332-AF91-4E3B-A485-6FAF93A58261}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19A48332-AF91-4E3B-A485-6FAF93A58261}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3164,7 +3164,7 @@
         <xdr:cNvPr id="57" name="CaixaDeTexto 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08033844-88BC-4D60-8FC9-0277B9368317}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08033844-88BC-4D60-8FC9-0277B9368317}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3222,7 +3222,7 @@
         <xdr:cNvPr id="58" name="CaixaDeTexto 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A90BA68C-9EA2-46A8-AB8F-787C61F09D76}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A90BA68C-9EA2-46A8-AB8F-787C61F09D76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3293,7 +3293,7 @@
         <xdr:cNvPr id="59" name="Retângulo 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5A1D37EE-2883-4E1B-A17D-03F345B623FC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A1D37EE-2883-4E1B-A17D-03F345B623FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3359,7 +3359,7 @@
         <xdr:cNvPr id="60" name="Retângulo 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ECA06E87-B0C9-49D5-9F4D-0D479D9DBBA0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECA06E87-B0C9-49D5-9F4D-0D479D9DBBA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3420,7 +3420,7 @@
         <xdr:cNvPr id="61" name="CaixaDeTexto 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{212C9E74-16F4-49FD-9373-5191CE86BF7C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{212C9E74-16F4-49FD-9373-5191CE86BF7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3478,7 +3478,7 @@
         <xdr:cNvPr id="62" name="CaixaDeTexto 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DB7072D2-8749-4802-9072-D7E98B58A978}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB7072D2-8749-4802-9072-D7E98B58A978}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3549,7 +3549,7 @@
         <xdr:cNvPr id="63" name="Retângulo 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8923E230-AD18-4029-A385-E0F91E90B63E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8923E230-AD18-4029-A385-E0F91E90B63E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3615,7 +3615,7 @@
         <xdr:cNvPr id="64" name="Retângulo 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{300581D6-E2A2-496F-967E-07B3D8CF8B0A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{300581D6-E2A2-496F-967E-07B3D8CF8B0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3676,7 +3676,7 @@
         <xdr:cNvPr id="65" name="CaixaDeTexto 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D4CEA790-D7B1-471E-BEB0-0B77A467A015}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4CEA790-D7B1-471E-BEB0-0B77A467A015}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3734,7 +3734,7 @@
         <xdr:cNvPr id="66" name="CaixaDeTexto 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF063CB1-452E-455E-AAD5-D84639351ABE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF063CB1-452E-455E-AAD5-D84639351ABE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3805,7 +3805,7 @@
         <xdr:cNvPr id="67" name="Retângulo 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E4F8495-FE03-43E0-8A38-6FF0E11BFFC2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E4F8495-FE03-43E0-8A38-6FF0E11BFFC2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3871,7 +3871,7 @@
         <xdr:cNvPr id="68" name="Retângulo 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A77388AB-A120-498B-953F-4FFEDEBAC1C6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A77388AB-A120-498B-953F-4FFEDEBAC1C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3937,7 +3937,7 @@
         <xdr:cNvPr id="69" name="Retângulo 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0881FB03-F5FA-4EB4-964D-82C5A230095F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0881FB03-F5FA-4EB4-964D-82C5A230095F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4003,7 +4003,7 @@
         <xdr:cNvPr id="70" name="Retângulo 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C12A09F1-57AB-4771-B731-F27D2226955A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C12A09F1-57AB-4771-B731-F27D2226955A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4069,7 +4069,7 @@
         <xdr:cNvPr id="71" name="Retângulo 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{30BEE643-6992-416E-9CFA-D7EC8EA54EA4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30BEE643-6992-416E-9CFA-D7EC8EA54EA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4135,7 +4135,7 @@
         <xdr:cNvPr id="72" name="Retângulo 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D4E86B9A-6F2D-46D7-B93D-25705B635B05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E86B9A-6F2D-46D7-B93D-25705B635B05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4201,7 +4201,7 @@
         <xdr:cNvPr id="73" name="Retângulo 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E65FCD74-3CB2-4218-81C0-17F665203FAE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E65FCD74-3CB2-4218-81C0-17F665203FAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4267,7 +4267,7 @@
         <xdr:cNvPr id="74" name="Retângulo 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BAE86BF7-FAD9-4D58-85E8-D5D283ED9AF1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAE86BF7-FAD9-4D58-85E8-D5D283ED9AF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4333,7 +4333,7 @@
         <xdr:cNvPr id="75" name="Retângulo 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B71C2CAE-18B0-49B1-B35D-1CF6283E3F93}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B71C2CAE-18B0-49B1-B35D-1CF6283E3F93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4399,7 +4399,7 @@
         <xdr:cNvPr id="76" name="Retângulo 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2339A59-5784-484A-8DCE-12988E5B57CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2339A59-5784-484A-8DCE-12988E5B57CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4465,7 +4465,7 @@
         <xdr:cNvPr id="77" name="Retângulo 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F25EFF5-A54E-40B0-BAB1-1C2F1E183620}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F25EFF5-A54E-40B0-BAB1-1C2F1E183620}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4531,7 +4531,7 @@
         <xdr:cNvPr id="78" name="Retângulo 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61EED6FA-92CE-4025-A64A-4A4DC542AF2C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61EED6FA-92CE-4025-A64A-4A4DC542AF2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4597,7 +4597,7 @@
         <xdr:cNvPr id="79" name="Retângulo 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CA4ABA14-CF36-4671-9FA9-A1DED49FD52D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA4ABA14-CF36-4671-9FA9-A1DED49FD52D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4663,7 +4663,7 @@
         <xdr:cNvPr id="80" name="Retângulo 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52520B53-743B-4EE1-B592-EDC652FBCBFF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52520B53-743B-4EE1-B592-EDC652FBCBFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4729,7 +4729,7 @@
         <xdr:cNvPr id="81" name="Retângulo 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78B0C140-605D-4377-BA38-8800A3884B44}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78B0C140-605D-4377-BA38-8800A3884B44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4795,7 +4795,7 @@
         <xdr:cNvPr id="82" name="Retângulo 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{37AE6197-41A3-4E5D-A4AF-0A475C4EAAE9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37AE6197-41A3-4E5D-A4AF-0A475C4EAAE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4861,7 +4861,7 @@
         <xdr:cNvPr id="83" name="Retângulo 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C606800-3B8F-4CDF-B8D2-FD01CD9D9138}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C606800-3B8F-4CDF-B8D2-FD01CD9D9138}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4927,7 +4927,7 @@
         <xdr:cNvPr id="84" name="Retângulo 83">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AFFD3051-031A-4105-A6B6-B51D1379FEA6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFFD3051-031A-4105-A6B6-B51D1379FEA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4993,7 +4993,7 @@
         <xdr:cNvPr id="85" name="Retângulo 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{275EFC6E-A962-4961-96D6-59996594462B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{275EFC6E-A962-4961-96D6-59996594462B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5059,7 +5059,7 @@
         <xdr:cNvPr id="86" name="Retângulo 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4649F0F1-F8E9-45DA-B109-CD1FD14AF5B3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4649F0F1-F8E9-45DA-B109-CD1FD14AF5B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5125,7 +5125,7 @@
         <xdr:cNvPr id="87" name="Retângulo 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E587C9C3-D767-4069-82CB-82A234D8EADF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E587C9C3-D767-4069-82CB-82A234D8EADF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5191,7 +5191,7 @@
         <xdr:cNvPr id="88" name="Retângulo 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BA38159B-71A5-4280-AC14-04EAC66F9B52}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA38159B-71A5-4280-AC14-04EAC66F9B52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5257,7 +5257,7 @@
         <xdr:cNvPr id="89" name="Retângulo 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AF070F4F-B1EB-4129-A94E-47719B915AC3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF070F4F-B1EB-4129-A94E-47719B915AC3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5323,7 +5323,7 @@
         <xdr:cNvPr id="90" name="Retângulo 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2D5DFBAC-40CD-4548-B5DD-5F9F6B7FE848}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D5DFBAC-40CD-4548-B5DD-5F9F6B7FE848}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5389,7 +5389,7 @@
         <xdr:cNvPr id="91" name="Retângulo 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F94B3A4A-D85D-4ACE-BEE9-0DC327A688F1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F94B3A4A-D85D-4ACE-BEE9-0DC327A688F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5455,7 +5455,7 @@
         <xdr:cNvPr id="92" name="Retângulo 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{12CFEDC9-0A31-4088-8B23-8B2747AECFF4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12CFEDC9-0A31-4088-8B23-8B2747AECFF4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5521,7 +5521,7 @@
         <xdr:cNvPr id="93" name="Retângulo 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D37B05FE-628B-4E31-9569-AD85F21BD6F7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D37B05FE-628B-4E31-9569-AD85F21BD6F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5587,7 +5587,7 @@
         <xdr:cNvPr id="94" name="Retângulo 93">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6B7C2A7C-4F6F-4998-BF47-458D72ECF5CC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B7C2A7C-4F6F-4998-BF47-458D72ECF5CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5653,7 +5653,7 @@
         <xdr:cNvPr id="95" name="Retângulo 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E722D203-8702-4C8C-9C45-CC751203BC29}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E722D203-8702-4C8C-9C45-CC751203BC29}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5719,7 +5719,7 @@
         <xdr:cNvPr id="104" name="Retângulo 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{177C7807-FB74-4C95-BB78-756922BC30AC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{177C7807-FB74-4C95-BB78-756922BC30AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5785,7 +5785,7 @@
         <xdr:cNvPr id="105" name="Retângulo 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E6FCFDD9-AD61-46F3-A9EF-1D1C0F188A07}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6FCFDD9-AD61-46F3-A9EF-1D1C0F188A07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5851,7 +5851,7 @@
         <xdr:cNvPr id="5" name="Seta: para a Direita 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD3C7F56-921F-41A8-874C-0103BD326E50}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD3C7F56-921F-41A8-874C-0103BD326E50}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5916,7 +5916,7 @@
         <xdr:cNvPr id="2" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91D9E789-2402-44BD-A1CC-A1C14D55B142}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91D9E789-2402-44BD-A1CC-A1C14D55B142}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5977,7 +5977,7 @@
         <xdr:cNvPr id="3" name="Retângulo 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{71FA2D94-2FE5-42D0-B061-81A34DC1F026}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71FA2D94-2FE5-42D0-B061-81A34DC1F026}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6043,7 +6043,7 @@
         <xdr:cNvPr id="4" name="Retângulo 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A740F65E-9A59-4C80-A788-532D8357C418}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A740F65E-9A59-4C80-A788-532D8357C418}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6104,7 +6104,7 @@
         <xdr:cNvPr id="5" name="CaixaDeTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{234CE881-34DB-4A8F-B322-B9C711DD370F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234CE881-34DB-4A8F-B322-B9C711DD370F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6162,7 +6162,7 @@
         <xdr:cNvPr id="6" name="CaixaDeTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F18597B-F4CD-4B63-AB0B-EA62284BF410}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F18597B-F4CD-4B63-AB0B-EA62284BF410}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6233,7 +6233,7 @@
         <xdr:cNvPr id="7" name="Retângulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08D41B6E-2B2F-488E-9CD6-BD82D0207693}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D41B6E-2B2F-488E-9CD6-BD82D0207693}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6299,7 +6299,7 @@
         <xdr:cNvPr id="8" name="Retângulo 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A26C5758-CFFF-427C-8C3C-7844DF494C58}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26C5758-CFFF-427C-8C3C-7844DF494C58}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6365,7 +6365,7 @@
         <xdr:cNvPr id="9" name="Retângulo 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1827BF8-045F-4D5D-8239-EFD3F0CFADAC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1827BF8-045F-4D5D-8239-EFD3F0CFADAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6426,7 +6426,7 @@
         <xdr:cNvPr id="10" name="CaixaDeTexto 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0490D997-3E32-43A5-BAD3-14A856B6C10F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0490D997-3E32-43A5-BAD3-14A856B6C10F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6484,7 +6484,7 @@
         <xdr:cNvPr id="11" name="CaixaDeTexto 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CB1ED0D2-600C-41C1-B8F4-E9FB224E5641}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB1ED0D2-600C-41C1-B8F4-E9FB224E5641}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6555,7 +6555,7 @@
         <xdr:cNvPr id="12" name="Retângulo 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD654C65-A4F0-4964-8EB7-3E0331B10E25}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD654C65-A4F0-4964-8EB7-3E0331B10E25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6621,7 +6621,7 @@
         <xdr:cNvPr id="13" name="Retângulo 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15B10A43-CC42-4E29-BDF6-055DB4E72038}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15B10A43-CC42-4E29-BDF6-055DB4E72038}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6682,7 +6682,7 @@
         <xdr:cNvPr id="14" name="CaixaDeTexto 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{68F19C26-7C20-45E8-B6F3-696266557732}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F19C26-7C20-45E8-B6F3-696266557732}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6740,7 +6740,7 @@
         <xdr:cNvPr id="15" name="CaixaDeTexto 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AA55FEAB-8B6F-4159-8116-3B6DDC6FDF75}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA55FEAB-8B6F-4159-8116-3B6DDC6FDF75}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6811,7 +6811,7 @@
         <xdr:cNvPr id="16" name="Retângulo 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8282E535-7FBC-4F9B-92F8-0DFA2D223597}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8282E535-7FBC-4F9B-92F8-0DFA2D223597}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6877,7 +6877,7 @@
         <xdr:cNvPr id="17" name="Retângulo 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6F985C8-0EBC-4496-B84F-3955A9516E0C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6F985C8-0EBC-4496-B84F-3955A9516E0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6938,7 +6938,7 @@
         <xdr:cNvPr id="18" name="CaixaDeTexto 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{321E4894-7E6D-4546-8DFC-9E5BF5CD9A86}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{321E4894-7E6D-4546-8DFC-9E5BF5CD9A86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6996,7 +6996,7 @@
         <xdr:cNvPr id="19" name="CaixaDeTexto 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{528D892E-6DC9-4789-A71D-4A8398B70F4C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{528D892E-6DC9-4789-A71D-4A8398B70F4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7067,7 +7067,7 @@
         <xdr:cNvPr id="20" name="Retângulo 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{821E4E71-FCFC-4841-B332-519FC8581706}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{821E4E71-FCFC-4841-B332-519FC8581706}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7133,7 +7133,7 @@
         <xdr:cNvPr id="21" name="Retângulo 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EDD86A36-D44B-4578-90E9-6C05C48E3C2C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDD86A36-D44B-4578-90E9-6C05C48E3C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7194,7 +7194,7 @@
         <xdr:cNvPr id="22" name="CaixaDeTexto 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CABAB187-A42A-4888-BA9B-D99120DCBC0B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CABAB187-A42A-4888-BA9B-D99120DCBC0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7252,7 +7252,7 @@
         <xdr:cNvPr id="23" name="CaixaDeTexto 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A80EF4FC-F3A3-42F7-B07A-1CC7D70F9E4D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80EF4FC-F3A3-42F7-B07A-1CC7D70F9E4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7323,7 +7323,7 @@
         <xdr:cNvPr id="24" name="Retângulo 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9692010B-3379-4C8D-8100-F16997E1C402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9692010B-3379-4C8D-8100-F16997E1C402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7389,7 +7389,7 @@
         <xdr:cNvPr id="25" name="Retângulo 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08DA8716-5356-4441-BD98-007724E0B260}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08DA8716-5356-4441-BD98-007724E0B260}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7450,7 +7450,7 @@
         <xdr:cNvPr id="26" name="CaixaDeTexto 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C0B0F513-5529-4448-B5FD-ABE21AD6E005}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0B0F513-5529-4448-B5FD-ABE21AD6E005}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7508,7 +7508,7 @@
         <xdr:cNvPr id="27" name="CaixaDeTexto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60F0D93E-948A-4E18-ADDD-560E49C871FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60F0D93E-948A-4E18-ADDD-560E49C871FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7579,7 +7579,7 @@
         <xdr:cNvPr id="28" name="Retângulo 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{308F178F-7772-44D2-A8C6-3500047FE8A8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{308F178F-7772-44D2-A8C6-3500047FE8A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7645,7 +7645,7 @@
         <xdr:cNvPr id="29" name="Retângulo 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{852513F3-6791-4546-AA2A-D531C98851B8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{852513F3-6791-4546-AA2A-D531C98851B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7711,7 +7711,7 @@
         <xdr:cNvPr id="30" name="Retângulo 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{347E82D1-4725-4640-8456-B6E8341988C7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{347E82D1-4725-4640-8456-B6E8341988C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7777,7 +7777,7 @@
         <xdr:cNvPr id="31" name="Retângulo 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7DCBE549-331F-4171-8E0D-85810134BEF1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DCBE549-331F-4171-8E0D-85810134BEF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7843,7 +7843,7 @@
         <xdr:cNvPr id="32" name="Retângulo 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D44767F-9CFB-4A4B-BFEE-554F906BE04F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D44767F-9CFB-4A4B-BFEE-554F906BE04F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7909,7 +7909,7 @@
         <xdr:cNvPr id="33" name="Retângulo 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F1C1515-63F1-4CAB-89A7-2051B4F98A0F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F1C1515-63F1-4CAB-89A7-2051B4F98A0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7975,7 +7975,7 @@
         <xdr:cNvPr id="34" name="Retângulo 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13AD6E3F-95BE-4EC2-A091-B34556D6F6EF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13AD6E3F-95BE-4EC2-A091-B34556D6F6EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8041,7 +8041,7 @@
         <xdr:cNvPr id="35" name="Retângulo 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE9224B5-14EE-4306-B34D-FAAEB01F37E3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9224B5-14EE-4306-B34D-FAAEB01F37E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8107,7 +8107,7 @@
         <xdr:cNvPr id="36" name="Retângulo 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CB4FC65E-CC3E-420B-84D5-C565CB1A6B4F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB4FC65E-CC3E-420B-84D5-C565CB1A6B4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8173,7 +8173,7 @@
         <xdr:cNvPr id="37" name="Retângulo 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A5FD2AD-71C9-4B69-9070-DEED0E80070A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A5FD2AD-71C9-4B69-9070-DEED0E80070A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8239,7 +8239,7 @@
         <xdr:cNvPr id="38" name="Retângulo 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4C5BC690-B245-4E57-B212-D00D65502295}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C5BC690-B245-4E57-B212-D00D65502295}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8305,7 +8305,7 @@
         <xdr:cNvPr id="39" name="Retângulo 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D595DFF-3C53-46FC-B71D-4688A085B127}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D595DFF-3C53-46FC-B71D-4688A085B127}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8371,7 +8371,7 @@
         <xdr:cNvPr id="40" name="Retângulo 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6A055816-2B6D-4D8C-B691-5B446D1140B5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A055816-2B6D-4D8C-B691-5B446D1140B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8437,7 +8437,7 @@
         <xdr:cNvPr id="41" name="Retângulo 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{27310266-29EF-403C-991D-348ADCF0A704}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27310266-29EF-403C-991D-348ADCF0A704}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8503,7 +8503,7 @@
         <xdr:cNvPr id="42" name="Retângulo 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D97A4628-F1E2-4518-B5DB-3137DB5CF5B2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D97A4628-F1E2-4518-B5DB-3137DB5CF5B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8569,7 +8569,7 @@
         <xdr:cNvPr id="43" name="Retângulo 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AAD09BF0-483E-4747-B1D4-8411057F7F08}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAD09BF0-483E-4747-B1D4-8411057F7F08}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8635,7 +8635,7 @@
         <xdr:cNvPr id="44" name="Retângulo 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C05D4AE0-330C-43D0-AF2D-450D841F14EA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C05D4AE0-330C-43D0-AF2D-450D841F14EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8701,7 +8701,7 @@
         <xdr:cNvPr id="45" name="Retângulo 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E6086E84-1631-4B9C-852F-7A473502F544}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6086E84-1631-4B9C-852F-7A473502F544}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8767,7 +8767,7 @@
         <xdr:cNvPr id="46" name="Retângulo 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B5BB088A-1F3D-44D8-ABE3-54C6B216820C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5BB088A-1F3D-44D8-ABE3-54C6B216820C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8833,7 +8833,7 @@
         <xdr:cNvPr id="59" name="Seta: para a Direita 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EBAE4820-D81E-4D27-9C06-C1F66BD428B2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBAE4820-D81E-4D27-9C06-C1F66BD428B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8893,7 +8893,7 @@
         <xdr:cNvPr id="60" name="Retângulo 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB53E992-CD1E-4AF5-A73A-44CE05129A93}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB53E992-CD1E-4AF5-A73A-44CE05129A93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8954,7 +8954,7 @@
         <xdr:cNvPr id="61" name="CaixaDeTexto 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D45DE83-10AF-4174-8220-728256A6F823}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D45DE83-10AF-4174-8220-728256A6F823}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9012,7 +9012,7 @@
         <xdr:cNvPr id="62" name="CaixaDeTexto 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{93C32CD6-5D10-40E2-B94B-5ED6AD9D1D01}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93C32CD6-5D10-40E2-B94B-5ED6AD9D1D01}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9083,7 +9083,7 @@
         <xdr:cNvPr id="63" name="Retângulo 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D2421441-EA4B-4100-A3C5-E7A04CF13139}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2421441-EA4B-4100-A3C5-E7A04CF13139}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9149,7 +9149,7 @@
         <xdr:cNvPr id="64" name="Retângulo 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{22A0EBE4-2C56-440A-835B-420348F8333A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22A0EBE4-2C56-440A-835B-420348F8333A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9210,7 +9210,7 @@
         <xdr:cNvPr id="65" name="CaixaDeTexto 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4C57BED5-CB2B-45BC-9F95-0ABD28F9D3E1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C57BED5-CB2B-45BC-9F95-0ABD28F9D3E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9268,7 +9268,7 @@
         <xdr:cNvPr id="66" name="CaixaDeTexto 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B467F391-8AF5-4D3A-998E-92AD37B84D49}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B467F391-8AF5-4D3A-998E-92AD37B84D49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9339,7 +9339,7 @@
         <xdr:cNvPr id="67" name="Retângulo 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6E11BC08-CEE0-4D40-8054-4A4A0C843040}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E11BC08-CEE0-4D40-8054-4A4A0C843040}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9690,7 +9690,7 @@
   <dimension ref="A1:O98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9709,68 +9709,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="109" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="133"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="111"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="134"/>
-      <c r="B2" s="135"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="136"/>
+      <c r="A2" s="112"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="114"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="138"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="116"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="139" t="s">
+      <c r="A4" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="140"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="145" t="s">
+      <c r="B4" s="118"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="146"/>
-      <c r="I4" s="197"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="89"/>
       <c r="J4" s="22"/>
       <c r="K4" s="78"/>
     </row>
@@ -9780,60 +9780,60 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="116"/>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
+      <c r="B6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="116"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
+      <c r="A7" s="124"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="93" t="s">
+      <c r="B8" s="163"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="163"/>
+      <c r="H8" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93" t="s">
+      <c r="I8" s="97"/>
+      <c r="J8" s="97" t="s">
         <v>123</v>
       </c>
-      <c r="K8" s="93"/>
+      <c r="K8" s="97"/>
     </row>
     <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="103"/>
-      <c r="B9" s="103"/>
-      <c r="C9" s="103"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="103"/>
+      <c r="A9" s="163"/>
+      <c r="B9" s="163"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="4" t="s">
         <v>18</v>
       </c>
@@ -9847,13 +9847,13 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="103"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="103"/>
+      <c r="A10" s="163"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="163"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="163"/>
       <c r="H10" s="4" t="s">
         <v>17</v>
       </c>
@@ -9864,13 +9864,13 @@
       <c r="K10" s="80"/>
     </row>
     <row r="11" spans="1:13" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="103"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
+      <c r="A11" s="163"/>
+      <c r="B11" s="163"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="163"/>
+      <c r="E11" s="163"/>
+      <c r="F11" s="163"/>
+      <c r="G11" s="163"/>
       <c r="H11" s="4" t="s">
         <v>106</v>
       </c>
@@ -9885,13 +9885,13 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="103"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
+      <c r="A12" s="163"/>
+      <c r="B12" s="163"/>
+      <c r="C12" s="163"/>
+      <c r="D12" s="163"/>
+      <c r="E12" s="163"/>
+      <c r="F12" s="163"/>
+      <c r="G12" s="163"/>
       <c r="H12" s="4" t="s">
         <v>107</v>
       </c>
@@ -9919,50 +9919,50 @@
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="156" t="s">
         <v>110</v>
       </c>
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="97" t="e">
+      <c r="B14" s="157"/>
+      <c r="C14" s="157"/>
+      <c r="D14" s="158"/>
+      <c r="E14" s="129" t="e">
         <f>VLOOKUP(J3,Dados!A:H,5,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F14" s="98"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="104" t="s">
+      <c r="F14" s="159"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="125" t="s">
         <v>121</v>
       </c>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104" t="s">
+      <c r="I14" s="125"/>
+      <c r="J14" s="125" t="s">
         <v>122</v>
       </c>
-      <c r="K14" s="104"/>
+      <c r="K14" s="125"/>
     </row>
     <row r="15" spans="1:13" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="156" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="95"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="96"/>
+      <c r="B15" s="157"/>
+      <c r="C15" s="157"/>
+      <c r="D15" s="157"/>
+      <c r="E15" s="157"/>
+      <c r="F15" s="157"/>
+      <c r="G15" s="157"/>
+      <c r="H15" s="157"/>
+      <c r="I15" s="157"/>
+      <c r="J15" s="157"/>
+      <c r="K15" s="158"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="102"/>
+      <c r="A16" s="160"/>
+      <c r="B16" s="161"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="161"/>
+      <c r="E16" s="161"/>
+      <c r="F16" s="161"/>
+      <c r="G16" s="162"/>
       <c r="H16" s="26" t="s">
         <v>2</v>
       </c>
@@ -9977,15 +9977,15 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="147"/>
-      <c r="B17" s="148"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="148"/>
-      <c r="E17" s="149"/>
-      <c r="F17" s="130" t="s">
+      <c r="A17" s="126"/>
+      <c r="B17" s="127"/>
+      <c r="C17" s="127"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="164" t="s">
         <v>125</v>
       </c>
-      <c r="G17" s="130"/>
+      <c r="G17" s="164"/>
       <c r="H17" s="29" t="e">
         <f>VLOOKUP(J3,Dados!A:N,14,0)</f>
         <v>#N/A</v>
@@ -10007,22 +10007,22 @@
       <c r="A18" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="B18" s="97" t="e">
+      <c r="B18" s="129" t="e">
         <f>VLOOKUP(J3,Dados!A:W,23,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="C18" s="99"/>
-      <c r="D18" s="159" t="s">
+      <c r="C18" s="130"/>
+      <c r="D18" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="E18" s="159" t="e">
+      <c r="E18" s="100" t="e">
         <f>VLOOKUP(J3,Dados!A:M,13,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="93"/>
+      <c r="G18" s="97"/>
       <c r="H18" s="2" t="e">
         <f>VLOOKUP(J3,Dados!A:P,16,0)</f>
         <v>#N/A</v>
@@ -10041,20 +10041,20 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="98" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="93" t="e">
+      <c r="B19" s="97" t="e">
         <f>VLOOKUP(J3,Dados!A:L,12,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="160"/>
-      <c r="E19" s="160"/>
-      <c r="F19" s="93" t="s">
+      <c r="C19" s="97"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="97" t="s">
         <v>229</v>
       </c>
-      <c r="G19" s="93"/>
+      <c r="G19" s="97"/>
       <c r="H19" s="2" t="e">
         <f>VLOOKUP(J3,Dados!A:R,18,0)</f>
         <v>#N/A</v>
@@ -10073,15 +10073,15 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="158"/>
-      <c r="B20" s="156"/>
-      <c r="C20" s="156"/>
-      <c r="D20" s="161"/>
-      <c r="E20" s="161"/>
-      <c r="F20" s="156" t="s">
+      <c r="A20" s="99"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="156"/>
+      <c r="G20" s="96"/>
       <c r="H20" s="32" t="e">
         <f>VLOOKUP(J3,Dados!A:T,20,0)</f>
         <v>#N/A</v>
@@ -10100,139 +10100,139 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="109" t="s">
+      <c r="A21" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="110"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="110"/>
-      <c r="E21" s="98" t="e">
+      <c r="B21" s="153"/>
+      <c r="C21" s="153"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="159" t="e">
         <f>VLOOKUP(J3,Dados!A1:F75,6,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F21" s="98"/>
-      <c r="G21" s="99"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="130"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
       <c r="K21" s="28"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="156" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="95"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="98" t="e">
+      <c r="B22" s="157"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="159" t="e">
         <f>VLOOKUP(J3,Dados!A:H,8,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F22" s="98"/>
-      <c r="G22" s="99"/>
+      <c r="F22" s="159"/>
+      <c r="G22" s="130"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="156" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="95"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="98" t="e">
+      <c r="B23" s="157"/>
+      <c r="C23" s="157"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="159" t="e">
         <f>VLOOKUP(J3,Dados!A:H,7,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F23" s="98"/>
-      <c r="G23" s="99"/>
-      <c r="H23" s="111"/>
-      <c r="I23" s="111"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="92"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="154"/>
+      <c r="I23" s="154"/>
+      <c r="J23" s="155"/>
+      <c r="K23" s="155"/>
     </row>
     <row r="24" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="112" t="s">
+      <c r="A25" s="131" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="113"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="113"/>
-      <c r="G25" s="113"/>
-      <c r="H25" s="113"/>
-      <c r="I25" s="113"/>
-      <c r="J25" s="113"/>
-      <c r="K25" s="114"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="132"/>
+      <c r="G25" s="132"/>
+      <c r="H25" s="132"/>
+      <c r="I25" s="132"/>
+      <c r="J25" s="132"/>
+      <c r="K25" s="133"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="115"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="116"/>
-      <c r="J26" s="116"/>
-      <c r="K26" s="117"/>
+      <c r="A26" s="134"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="124"/>
+      <c r="K26" s="135"/>
     </row>
     <row r="27" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="121" t="s">
+      <c r="A27" s="139" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="122"/>
-      <c r="H27" s="122" t="s">
+      <c r="B27" s="140"/>
+      <c r="C27" s="140"/>
+      <c r="D27" s="140"/>
+      <c r="E27" s="140"/>
+      <c r="F27" s="140"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="140" t="s">
         <v>117</v>
       </c>
-      <c r="I27" s="122"/>
-      <c r="J27" s="122"/>
-      <c r="K27" s="123"/>
+      <c r="I27" s="140"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="141"/>
     </row>
     <row r="28" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="136" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="119"/>
-      <c r="C28" s="119"/>
-      <c r="D28" s="119"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="119" t="s">
+      <c r="B28" s="137"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="137"/>
+      <c r="G28" s="137"/>
+      <c r="H28" s="137" t="s">
         <v>186</v>
       </c>
-      <c r="I28" s="119"/>
-      <c r="J28" s="119"/>
-      <c r="K28" s="120"/>
+      <c r="I28" s="137"/>
+      <c r="J28" s="137"/>
+      <c r="K28" s="138"/>
     </row>
     <row r="29" spans="1:15" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
     </row>
     <row r="30" spans="1:15" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="124" t="s">
+      <c r="A30" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="125"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="125"/>
-      <c r="E30" s="125"/>
-      <c r="F30" s="125"/>
-      <c r="G30" s="125"/>
-      <c r="H30" s="125"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="125"/>
-      <c r="K30" s="126"/>
+      <c r="B30" s="143"/>
+      <c r="C30" s="143"/>
+      <c r="D30" s="143"/>
+      <c r="E30" s="143"/>
+      <c r="F30" s="143"/>
+      <c r="G30" s="143"/>
+      <c r="H30" s="143"/>
+      <c r="I30" s="143"/>
+      <c r="J30" s="143"/>
+      <c r="K30" s="144"/>
       <c r="O30" t="s">
         <v>16</v>
       </c>
@@ -10243,16 +10243,16 @@
       </c>
     </row>
     <row r="33" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="127" t="s">
+      <c r="A33" s="145" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="128"/>
-      <c r="C33" s="128"/>
-      <c r="D33" s="128"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="105"/>
-      <c r="H33" s="105"/>
+      <c r="B33" s="146"/>
+      <c r="C33" s="146"/>
+      <c r="D33" s="146"/>
+      <c r="E33" s="147"/>
+      <c r="F33" s="151"/>
+      <c r="G33" s="151"/>
+      <c r="H33" s="151"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9" t="s">
         <v>12</v>
@@ -10263,16 +10263,16 @@
     </row>
     <row r="34" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="89">
+      <c r="A35" s="148">
         <v>1</v>
       </c>
-      <c r="B35" s="90"/>
-      <c r="C35" s="90"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="106"/>
-      <c r="G35" s="107"/>
-      <c r="H35" s="108"/>
+      <c r="B35" s="149"/>
+      <c r="C35" s="149"/>
+      <c r="D35" s="149"/>
+      <c r="E35" s="150"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="105"/>
       <c r="I35" s="83"/>
       <c r="J35" s="8" t="s">
         <v>118</v>
@@ -10280,16 +10280,16 @@
       <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="89">
+      <c r="A36" s="148">
         <v>2</v>
       </c>
-      <c r="B36" s="90"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="91"/>
-      <c r="F36" s="106"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="108"/>
+      <c r="B36" s="149"/>
+      <c r="C36" s="149"/>
+      <c r="D36" s="149"/>
+      <c r="E36" s="150"/>
+      <c r="F36" s="103"/>
+      <c r="G36" s="104"/>
+      <c r="H36" s="105"/>
       <c r="I36" s="83"/>
       <c r="J36" s="8" t="s">
         <v>118</v>
@@ -10297,16 +10297,16 @@
       <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="89">
+      <c r="A37" s="148">
         <v>3</v>
       </c>
-      <c r="B37" s="90"/>
-      <c r="C37" s="90"/>
-      <c r="D37" s="90"/>
-      <c r="E37" s="91"/>
-      <c r="F37" s="106"/>
-      <c r="G37" s="107"/>
-      <c r="H37" s="108"/>
+      <c r="B37" s="149"/>
+      <c r="C37" s="149"/>
+      <c r="D37" s="149"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="104"/>
+      <c r="H37" s="105"/>
       <c r="I37" s="83"/>
       <c r="J37" s="8" t="s">
         <v>118</v>
@@ -10314,16 +10314,16 @@
       <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="89">
+      <c r="A38" s="148">
         <v>4</v>
       </c>
-      <c r="B38" s="90"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="90"/>
-      <c r="E38" s="91"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="107"/>
-      <c r="H38" s="108"/>
+      <c r="B38" s="149"/>
+      <c r="C38" s="149"/>
+      <c r="D38" s="149"/>
+      <c r="E38" s="150"/>
+      <c r="F38" s="103"/>
+      <c r="G38" s="104"/>
+      <c r="H38" s="105"/>
       <c r="I38" s="83"/>
       <c r="J38" s="8" t="s">
         <v>118</v>
@@ -10331,16 +10331,16 @@
       <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="89">
+      <c r="A39" s="148">
         <v>5</v>
       </c>
-      <c r="B39" s="90"/>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="91"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="107"/>
-      <c r="H39" s="108"/>
+      <c r="B39" s="149"/>
+      <c r="C39" s="149"/>
+      <c r="D39" s="149"/>
+      <c r="E39" s="150"/>
+      <c r="F39" s="103"/>
+      <c r="G39" s="104"/>
+      <c r="H39" s="105"/>
       <c r="I39" s="83"/>
       <c r="J39" s="8" t="s">
         <v>118</v>
@@ -10348,16 +10348,16 @@
       <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="89">
+      <c r="A40" s="148">
         <v>6</v>
       </c>
-      <c r="B40" s="90"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="90"/>
-      <c r="E40" s="91"/>
-      <c r="F40" s="106"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="108"/>
+      <c r="B40" s="149"/>
+      <c r="C40" s="149"/>
+      <c r="D40" s="149"/>
+      <c r="E40" s="150"/>
+      <c r="F40" s="103"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="105"/>
       <c r="I40" s="83"/>
       <c r="J40" s="8" t="s">
         <v>118</v>
@@ -10365,16 +10365,16 @@
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="89">
+      <c r="A41" s="148">
         <v>7</v>
       </c>
-      <c r="B41" s="90"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-      <c r="E41" s="91"/>
-      <c r="F41" s="106"/>
-      <c r="G41" s="107"/>
-      <c r="H41" s="108"/>
+      <c r="B41" s="149"/>
+      <c r="C41" s="149"/>
+      <c r="D41" s="149"/>
+      <c r="E41" s="150"/>
+      <c r="F41" s="103"/>
+      <c r="G41" s="104"/>
+      <c r="H41" s="105"/>
       <c r="I41" s="83"/>
       <c r="J41" s="8" t="s">
         <v>118</v>
@@ -10382,16 +10382,16 @@
       <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="89">
+      <c r="A42" s="148">
         <v>8</v>
       </c>
-      <c r="B42" s="90"/>
-      <c r="C42" s="90"/>
-      <c r="D42" s="90"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="106"/>
-      <c r="G42" s="107"/>
-      <c r="H42" s="108"/>
+      <c r="B42" s="149"/>
+      <c r="C42" s="149"/>
+      <c r="D42" s="149"/>
+      <c r="E42" s="150"/>
+      <c r="F42" s="103"/>
+      <c r="G42" s="104"/>
+      <c r="H42" s="105"/>
       <c r="I42" s="83"/>
       <c r="J42" s="8" t="s">
         <v>118</v>
@@ -10399,16 +10399,16 @@
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="89">
+      <c r="A43" s="148">
         <v>9</v>
       </c>
-      <c r="B43" s="90"/>
-      <c r="C43" s="90"/>
-      <c r="D43" s="90"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="106"/>
-      <c r="G43" s="107"/>
-      <c r="H43" s="108"/>
+      <c r="B43" s="149"/>
+      <c r="C43" s="149"/>
+      <c r="D43" s="149"/>
+      <c r="E43" s="150"/>
+      <c r="F43" s="103"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="105"/>
       <c r="I43" s="83"/>
       <c r="J43" s="8" t="s">
         <v>118</v>
@@ -10416,16 +10416,16 @@
       <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="89">
+      <c r="A44" s="148">
         <v>10</v>
       </c>
-      <c r="B44" s="90"/>
-      <c r="C44" s="90"/>
-      <c r="D44" s="90"/>
-      <c r="E44" s="91"/>
-      <c r="F44" s="106"/>
-      <c r="G44" s="107"/>
-      <c r="H44" s="108"/>
+      <c r="B44" s="149"/>
+      <c r="C44" s="149"/>
+      <c r="D44" s="149"/>
+      <c r="E44" s="150"/>
+      <c r="F44" s="103"/>
+      <c r="G44" s="104"/>
+      <c r="H44" s="105"/>
       <c r="I44" s="83"/>
       <c r="J44" s="8" t="s">
         <v>118</v>
@@ -10433,16 +10433,16 @@
       <c r="K44" s="5"/>
     </row>
     <row r="45" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="89">
+      <c r="A45" s="148">
         <v>11</v>
       </c>
-      <c r="B45" s="90"/>
-      <c r="C45" s="90"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="106"/>
-      <c r="G45" s="107"/>
-      <c r="H45" s="108"/>
+      <c r="B45" s="149"/>
+      <c r="C45" s="149"/>
+      <c r="D45" s="149"/>
+      <c r="E45" s="150"/>
+      <c r="F45" s="103"/>
+      <c r="G45" s="104"/>
+      <c r="H45" s="105"/>
       <c r="I45" s="83"/>
       <c r="J45" s="8" t="s">
         <v>118</v>
@@ -10450,16 +10450,16 @@
       <c r="K45" s="5"/>
     </row>
     <row r="46" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="89">
+      <c r="A46" s="148">
         <v>12</v>
       </c>
-      <c r="B46" s="90"/>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="91"/>
-      <c r="F46" s="163"/>
-      <c r="G46" s="163"/>
-      <c r="H46" s="163"/>
+      <c r="B46" s="149"/>
+      <c r="C46" s="149"/>
+      <c r="D46" s="149"/>
+      <c r="E46" s="150"/>
+      <c r="F46" s="107"/>
+      <c r="G46" s="107"/>
+      <c r="H46" s="107"/>
       <c r="I46" s="83"/>
       <c r="J46" s="8" t="s">
         <v>118</v>
@@ -10467,16 +10467,16 @@
       <c r="K46" s="5"/>
     </row>
     <row r="47" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="89">
+      <c r="A47" s="148">
         <v>13</v>
       </c>
-      <c r="B47" s="90"/>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="163"/>
-      <c r="G47" s="163"/>
-      <c r="H47" s="163"/>
+      <c r="B47" s="149"/>
+      <c r="C47" s="149"/>
+      <c r="D47" s="149"/>
+      <c r="E47" s="150"/>
+      <c r="F47" s="107"/>
+      <c r="G47" s="107"/>
+      <c r="H47" s="107"/>
       <c r="I47" s="81"/>
       <c r="J47" s="8" t="s">
         <v>118</v>
@@ -10484,16 +10484,16 @@
       <c r="K47" s="5"/>
     </row>
     <row r="48" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="89">
+      <c r="A48" s="148">
         <v>14</v>
       </c>
-      <c r="B48" s="90"/>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="91"/>
-      <c r="F48" s="163"/>
-      <c r="G48" s="163"/>
-      <c r="H48" s="163"/>
+      <c r="B48" s="149"/>
+      <c r="C48" s="149"/>
+      <c r="D48" s="149"/>
+      <c r="E48" s="150"/>
+      <c r="F48" s="107"/>
+      <c r="G48" s="107"/>
+      <c r="H48" s="107"/>
       <c r="I48" s="81"/>
       <c r="J48" s="8" t="s">
         <v>118</v>
@@ -10501,16 +10501,16 @@
       <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:11" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="89">
+      <c r="A49" s="148">
         <v>15</v>
       </c>
-      <c r="B49" s="90"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="163"/>
-      <c r="G49" s="163"/>
-      <c r="H49" s="163"/>
+      <c r="B49" s="149"/>
+      <c r="C49" s="149"/>
+      <c r="D49" s="149"/>
+      <c r="E49" s="150"/>
+      <c r="F49" s="107"/>
+      <c r="G49" s="107"/>
+      <c r="H49" s="107"/>
       <c r="I49" s="81"/>
       <c r="J49" s="8" t="s">
         <v>118</v>
@@ -10519,60 +10519,60 @@
     </row>
     <row r="50" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
-      <c r="B50" s="162"/>
-      <c r="C50" s="162"/>
-      <c r="D50" s="162"/>
-      <c r="E50" s="162"/>
-      <c r="F50" s="162"/>
-      <c r="G50" s="162"/>
-      <c r="H50" s="162"/>
+      <c r="B50" s="106"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="106"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="106"/>
+      <c r="H50" s="106"/>
       <c r="I50" s="88"/>
       <c r="J50" s="7"/>
       <c r="K50" s="25"/>
     </row>
     <row r="51" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="164" t="s">
+      <c r="A51" s="108" t="s">
         <v>120</v>
       </c>
-      <c r="B51" s="164"/>
-      <c r="C51" s="164"/>
-      <c r="D51" s="164"/>
-      <c r="E51" s="164"/>
-      <c r="F51" s="164"/>
-      <c r="G51" s="164"/>
-      <c r="H51" s="164"/>
-      <c r="I51" s="164"/>
-      <c r="J51" s="164"/>
-      <c r="K51" s="164"/>
+      <c r="B51" s="108"/>
+      <c r="C51" s="108"/>
+      <c r="D51" s="108"/>
+      <c r="E51" s="108"/>
+      <c r="F51" s="108"/>
+      <c r="G51" s="108"/>
+      <c r="H51" s="108"/>
+      <c r="I51" s="108"/>
+      <c r="J51" s="108"/>
+      <c r="K51" s="108"/>
     </row>
     <row r="52" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="150" t="s">
+      <c r="A53" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="151"/>
-      <c r="C53" s="151"/>
-      <c r="D53" s="151"/>
-      <c r="E53" s="151"/>
-      <c r="F53" s="151"/>
-      <c r="G53" s="151"/>
-      <c r="H53" s="151"/>
-      <c r="I53" s="151"/>
-      <c r="J53" s="151"/>
-      <c r="K53" s="152"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="91"/>
+      <c r="E53" s="91"/>
+      <c r="F53" s="91"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="91"/>
+      <c r="J53" s="91"/>
+      <c r="K53" s="92"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="153"/>
-      <c r="B54" s="154"/>
-      <c r="C54" s="154"/>
-      <c r="D54" s="154"/>
-      <c r="E54" s="154"/>
-      <c r="F54" s="154"/>
-      <c r="G54" s="154"/>
-      <c r="H54" s="154"/>
-      <c r="I54" s="154"/>
-      <c r="J54" s="154"/>
-      <c r="K54" s="155"/>
+      <c r="A54" s="93"/>
+      <c r="B54" s="94"/>
+      <c r="C54" s="94"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="94"/>
+      <c r="F54" s="94"/>
+      <c r="G54" s="94"/>
+      <c r="H54" s="94"/>
+      <c r="I54" s="94"/>
+      <c r="J54" s="94"/>
+      <c r="K54" s="95"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="85" t="s">
@@ -10606,6 +10606,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A8:G12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="A25:K26"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A6:K7"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="A53:K54"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="B19:C20"/>
@@ -10622,68 +10684,6 @@
     <mergeCell ref="F48:H48"/>
     <mergeCell ref="F46:H46"/>
     <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A6:K7"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="A25:K26"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A8:G12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E48"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -16289,72 +16289,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="109" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="133"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="111"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="134"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="136"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="114"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="139" t="s">
+      <c r="C3" s="118"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="141"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="145">
+      <c r="I3" s="119"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="122">
         <v>4236654</v>
       </c>
-      <c r="L3" s="184"/>
+      <c r="L3" s="180"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="62"/>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="140"/>
-      <c r="D4" s="185"/>
-      <c r="E4" s="185"/>
-      <c r="F4" s="185"/>
-      <c r="G4" s="186"/>
-      <c r="H4" s="145" t="s">
+      <c r="C4" s="118"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="146"/>
+      <c r="I4" s="123"/>
       <c r="J4" s="23"/>
       <c r="K4" s="22" t="s">
         <v>105</v>
@@ -16363,32 +16363,32 @@
     </row>
     <row r="5" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="116" t="s">
+      <c r="B6" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="116"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="116"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="68" t="s">
@@ -16400,14 +16400,14 @@
       <c r="F8" s="68"/>
       <c r="G8" s="68"/>
       <c r="H8" s="68"/>
-      <c r="I8" s="93" t="s">
+      <c r="I8" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93" t="s">
+      <c r="J8" s="97"/>
+      <c r="K8" s="97" t="s">
         <v>123</v>
       </c>
-      <c r="L8" s="93"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="68"/>
@@ -16431,11 +16431,11 @@
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
       <c r="E10" s="68"/>
-      <c r="F10" s="97" t="s">
+      <c r="F10" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="98"/>
-      <c r="H10" s="99"/>
+      <c r="G10" s="159"/>
+      <c r="H10" s="130"/>
       <c r="I10" s="46"/>
       <c r="J10" s="36"/>
       <c r="K10" s="4" t="s">
@@ -16448,11 +16448,11 @@
       <c r="C11" s="68"/>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
-      <c r="F11" s="97" t="s">
+      <c r="F11" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="98"/>
-      <c r="H11" s="99"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="130"/>
       <c r="I11" s="46"/>
       <c r="J11" s="36"/>
       <c r="K11" s="4" t="s">
@@ -16465,11 +16465,11 @@
       <c r="C12" s="68"/>
       <c r="D12" s="68"/>
       <c r="E12" s="68"/>
-      <c r="F12" s="97" t="s">
+      <c r="F12" s="129" t="s">
         <v>106</v>
       </c>
-      <c r="G12" s="98"/>
-      <c r="H12" s="99"/>
+      <c r="G12" s="159"/>
+      <c r="H12" s="130"/>
       <c r="I12" s="24" t="s">
         <v>108</v>
       </c>
@@ -16488,11 +16488,11 @@
       <c r="C13" s="68"/>
       <c r="D13" s="68"/>
       <c r="E13" s="68"/>
-      <c r="F13" s="97" t="s">
+      <c r="F13" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="98"/>
-      <c r="H13" s="99"/>
+      <c r="G13" s="159"/>
+      <c r="H13" s="130"/>
       <c r="I13" s="24" t="s">
         <v>108</v>
       </c>
@@ -16520,69 +16520,69 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="156" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97" t="str">
+      <c r="C15" s="157"/>
+      <c r="D15" s="157"/>
+      <c r="E15" s="158"/>
+      <c r="F15" s="129" t="str">
         <f>VLOOKUP(K3,Dados!A:H,5,0)</f>
         <v>35 a 50 psi</v>
       </c>
-      <c r="G15" s="98"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="104" t="s">
+      <c r="G15" s="159"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="125" t="s">
         <v>121</v>
       </c>
-      <c r="J15" s="104"/>
-      <c r="K15" s="104" t="s">
+      <c r="J15" s="125"/>
+      <c r="K15" s="125" t="s">
         <v>122</v>
       </c>
-      <c r="L15" s="104"/>
+      <c r="L15" s="125"/>
     </row>
     <row r="16" spans="1:14" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="94" t="s">
+      <c r="B16" s="156" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="102"/>
+      <c r="C16" s="157"/>
+      <c r="D16" s="157"/>
+      <c r="E16" s="157"/>
+      <c r="F16" s="157"/>
+      <c r="G16" s="157"/>
+      <c r="H16" s="157"/>
+      <c r="I16" s="161"/>
+      <c r="J16" s="161"/>
+      <c r="K16" s="161"/>
+      <c r="L16" s="162"/>
     </row>
     <row r="17" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="100"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="101"/>
-      <c r="I17" s="187" t="s">
+      <c r="B17" s="160"/>
+      <c r="C17" s="161"/>
+      <c r="D17" s="161"/>
+      <c r="E17" s="161"/>
+      <c r="F17" s="161"/>
+      <c r="G17" s="161"/>
+      <c r="H17" s="161"/>
+      <c r="I17" s="178" t="s">
         <v>187</v>
       </c>
-      <c r="J17" s="188"/>
-      <c r="K17" s="187" t="s">
+      <c r="J17" s="179"/>
+      <c r="K17" s="178" t="s">
         <v>187</v>
       </c>
-      <c r="L17" s="188"/>
+      <c r="L17" s="179"/>
     </row>
     <row r="18" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="170" t="s">
+      <c r="B18" s="174" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="130"/>
-      <c r="D18" s="130"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="171"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="164"/>
+      <c r="H18" s="181"/>
       <c r="I18" s="39" t="s">
         <v>2</v>
       </c>
@@ -16597,20 +16597,20 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="157" t="s">
+      <c r="B19" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="65" t="str">
         <f>VLOOKUP(K3,Dados!A:AF,5,0)</f>
         <v>35 a 50 psi</v>
       </c>
-      <c r="G19" s="93" t="s">
+      <c r="G19" s="97" t="s">
         <v>125</v>
       </c>
-      <c r="H19" s="181"/>
+      <c r="H19" s="169"/>
       <c r="I19" s="54" t="str">
         <f>VLOOKUP(K3,Dados!A:N,14,0)</f>
         <v>____:____</v>
@@ -16629,10 +16629,10 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="172" t="s">
+      <c r="B20" s="182" t="s">
         <v>189</v>
       </c>
-      <c r="C20" s="159"/>
+      <c r="C20" s="100"/>
       <c r="D20" s="67">
         <f>VLOOKUP(K3,Dados!A:O,12,0)</f>
         <v>1</v>
@@ -16644,10 +16644,10 @@
         <f>VLOOKUP(K3,Dados!A:M,13,0)</f>
         <v>N/A</v>
       </c>
-      <c r="G20" s="159" t="s">
+      <c r="G20" s="100" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="196"/>
+      <c r="H20" s="170"/>
       <c r="I20" s="53" t="str">
         <f>VLOOKUP(K3,Dados!A:P,16,0)</f>
         <v>N/A</v>
@@ -16666,58 +16666,58 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="186" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="177"/>
-      <c r="D21" s="177"/>
-      <c r="E21" s="177"/>
-      <c r="F21" s="130" t="str">
+      <c r="C21" s="187"/>
+      <c r="D21" s="187"/>
+      <c r="E21" s="187"/>
+      <c r="F21" s="164" t="str">
         <f>VLOOKUP(K3,Dados!A:L,6,0)</f>
         <v>15 min./ Mínimo</v>
       </c>
-      <c r="G21" s="130"/>
-      <c r="H21" s="178"/>
+      <c r="G21" s="164"/>
+      <c r="H21" s="175"/>
       <c r="I21" s="61"/>
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="63"/>
     </row>
     <row r="22" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="179" t="s">
+      <c r="B22" s="188" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="180"/>
-      <c r="D22" s="180"/>
-      <c r="E22" s="180"/>
-      <c r="F22" s="93" t="str">
+      <c r="C22" s="189"/>
+      <c r="D22" s="189"/>
+      <c r="E22" s="189"/>
+      <c r="F22" s="97" t="str">
         <f>VLOOKUP(K3,Dados!A:H,8,0)</f>
         <v>120 min./ Mínimo</v>
       </c>
-      <c r="G22" s="93"/>
-      <c r="H22" s="181"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="169"/>
       <c r="I22" s="52"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="64"/>
     </row>
     <row r="23" spans="2:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="182" t="s">
+      <c r="B23" s="190" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="183"/>
-      <c r="D23" s="183"/>
-      <c r="E23" s="183"/>
-      <c r="F23" s="156" t="str">
+      <c r="C23" s="191"/>
+      <c r="D23" s="191"/>
+      <c r="E23" s="191"/>
+      <c r="F23" s="96" t="str">
         <f>VLOOKUP(K3,Dados!A:J,7,0)</f>
         <v>60ºC</v>
       </c>
-      <c r="G23" s="156"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="192"/>
-      <c r="J23" s="193"/>
-      <c r="K23" s="194"/>
-      <c r="L23" s="195"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="183"/>
+      <c r="I23" s="165"/>
+      <c r="J23" s="166"/>
+      <c r="K23" s="167"/>
+      <c r="L23" s="168"/>
     </row>
     <row r="24" spans="2:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="48"/>
@@ -16733,32 +16733,32 @@
       <c r="L24" s="51"/>
     </row>
     <row r="25" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="191"/>
-      <c r="C25" s="191"/>
-      <c r="D25" s="191"/>
-      <c r="E25" s="191"/>
+      <c r="B25" s="173"/>
+      <c r="C25" s="173"/>
+      <c r="D25" s="173"/>
+      <c r="E25" s="173"/>
       <c r="F25" s="50"/>
-      <c r="G25" s="191"/>
-      <c r="H25" s="191"/>
-      <c r="I25" s="189" t="s">
+      <c r="G25" s="173"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="171" t="s">
         <v>191</v>
       </c>
-      <c r="J25" s="190"/>
-      <c r="K25" s="189" t="s">
+      <c r="J25" s="172"/>
+      <c r="K25" s="171" t="s">
         <v>191</v>
       </c>
-      <c r="L25" s="190"/>
+      <c r="L25" s="172"/>
     </row>
     <row r="26" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="170" t="s">
+      <c r="B26" s="174" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="130"/>
-      <c r="D26" s="130"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="130"/>
-      <c r="G26" s="130"/>
-      <c r="H26" s="178"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="164"/>
+      <c r="H26" s="175"/>
       <c r="I26" s="59" t="s">
         <v>2</v>
       </c>
@@ -16773,20 +16773,20 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="157" t="s">
+      <c r="B27" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="93"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
       <c r="F27" s="72">
         <f>VLOOKUP(K3,Dados!A:Y,25,0)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="167" t="s">
+      <c r="G27" s="192" t="s">
         <v>125</v>
       </c>
-      <c r="H27" s="168"/>
+      <c r="H27" s="193"/>
       <c r="I27" s="61">
         <f>VLOOKUP(K3,Dados!A:AE,26,0)</f>
         <v>0</v>
@@ -16805,10 +16805,10 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="169" t="s">
+      <c r="B28" s="194" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="161"/>
+      <c r="C28" s="102"/>
       <c r="D28" s="73">
         <f>VLOOKUP(K3,Dados!A:AE,31,0)</f>
         <v>0</v>
@@ -16820,10 +16820,10 @@
         <f>VLOOKUP(K3,Dados!A:AF,24,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="156" t="s">
+      <c r="G28" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="H28" s="173"/>
+      <c r="H28" s="183"/>
       <c r="I28" s="53" t="str">
         <f>VLOOKUP(K3,Dados!A:T,20,0)</f>
         <v>N/A</v>
@@ -16842,139 +16842,139 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="109" t="s">
+      <c r="B29" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="110"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="110"/>
-      <c r="F29" s="174" t="str">
+      <c r="C29" s="153"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="153"/>
+      <c r="F29" s="184" t="str">
         <f>VLOOKUP(K3,Dados!A:H,6,0)</f>
         <v>15 min./ Mínimo</v>
       </c>
-      <c r="G29" s="174"/>
-      <c r="H29" s="175"/>
+      <c r="G29" s="184"/>
+      <c r="H29" s="185"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
       <c r="L29" s="28"/>
     </row>
     <row r="30" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="156" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="98" t="str">
+      <c r="C30" s="157"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="157"/>
+      <c r="F30" s="159" t="str">
         <f>VLOOKUP(K3,Dados!A:H,8,0)</f>
         <v>120 min./ Mínimo</v>
       </c>
-      <c r="G30" s="98"/>
-      <c r="H30" s="99"/>
+      <c r="G30" s="159"/>
+      <c r="H30" s="130"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="156" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="98" t="str">
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="159" t="str">
         <f>VLOOKUP(K3,Dados!A:H,7,0)</f>
         <v>60ºC</v>
       </c>
-      <c r="G31" s="98"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="111"/>
-      <c r="J31" s="111"/>
-      <c r="K31" s="92"/>
-      <c r="L31" s="92"/>
+      <c r="G31" s="159"/>
+      <c r="H31" s="130"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="154"/>
+      <c r="K31" s="155"/>
+      <c r="L31" s="155"/>
     </row>
     <row r="32" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="112" t="s">
+      <c r="B33" s="131" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="113"/>
-      <c r="D33" s="113"/>
-      <c r="E33" s="113"/>
-      <c r="F33" s="113"/>
-      <c r="G33" s="113"/>
-      <c r="H33" s="113"/>
-      <c r="I33" s="113"/>
-      <c r="J33" s="113"/>
-      <c r="K33" s="113"/>
-      <c r="L33" s="114"/>
+      <c r="C33" s="132"/>
+      <c r="D33" s="132"/>
+      <c r="E33" s="132"/>
+      <c r="F33" s="132"/>
+      <c r="G33" s="132"/>
+      <c r="H33" s="132"/>
+      <c r="I33" s="132"/>
+      <c r="J33" s="132"/>
+      <c r="K33" s="132"/>
+      <c r="L33" s="133"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="115"/>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="116"/>
-      <c r="L34" s="117"/>
+      <c r="B34" s="134"/>
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="124"/>
+      <c r="H34" s="124"/>
+      <c r="I34" s="124"/>
+      <c r="J34" s="124"/>
+      <c r="K34" s="124"/>
+      <c r="L34" s="135"/>
     </row>
     <row r="35" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="121" t="s">
+      <c r="B35" s="139" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="122"/>
-      <c r="D35" s="122"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="122"/>
-      <c r="G35" s="122"/>
-      <c r="H35" s="122"/>
-      <c r="I35" s="122" t="s">
+      <c r="C35" s="140"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="140"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="140"/>
+      <c r="I35" s="140" t="s">
         <v>117</v>
       </c>
-      <c r="J35" s="122"/>
-      <c r="K35" s="122"/>
-      <c r="L35" s="123"/>
+      <c r="J35" s="140"/>
+      <c r="K35" s="140"/>
+      <c r="L35" s="141"/>
     </row>
     <row r="36" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="118" t="s">
+      <c r="B36" s="136" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="119"/>
-      <c r="D36" s="119"/>
-      <c r="E36" s="119"/>
-      <c r="F36" s="119"/>
-      <c r="G36" s="119"/>
-      <c r="H36" s="119"/>
-      <c r="I36" s="119" t="s">
+      <c r="C36" s="137"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="137"/>
+      <c r="G36" s="137"/>
+      <c r="H36" s="137"/>
+      <c r="I36" s="137" t="s">
         <v>116</v>
       </c>
-      <c r="J36" s="119"/>
-      <c r="K36" s="119"/>
-      <c r="L36" s="120"/>
+      <c r="J36" s="137"/>
+      <c r="K36" s="137"/>
+      <c r="L36" s="138"/>
     </row>
     <row r="37" spans="1:16" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
     </row>
     <row r="38" spans="1:16" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="124" t="s">
+      <c r="B38" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="125"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="125"/>
-      <c r="F38" s="125"/>
-      <c r="G38" s="125"/>
-      <c r="H38" s="125"/>
-      <c r="I38" s="125"/>
-      <c r="J38" s="125"/>
-      <c r="K38" s="125"/>
-      <c r="L38" s="126"/>
+      <c r="C38" s="143"/>
+      <c r="D38" s="143"/>
+      <c r="E38" s="143"/>
+      <c r="F38" s="143"/>
+      <c r="G38" s="143"/>
+      <c r="H38" s="143"/>
+      <c r="I38" s="143"/>
+      <c r="J38" s="143"/>
+      <c r="K38" s="143"/>
+      <c r="L38" s="144"/>
       <c r="P38" t="s">
         <v>16</v>
       </c>
@@ -16989,17 +16989,17 @@
       <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="127" t="s">
+      <c r="C41" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="128"/>
-      <c r="E41" s="128"/>
-      <c r="F41" s="129"/>
-      <c r="G41" s="105" t="s">
+      <c r="D41" s="146"/>
+      <c r="E41" s="146"/>
+      <c r="F41" s="147"/>
+      <c r="G41" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="105"/>
-      <c r="I41" s="105"/>
+      <c r="H41" s="151"/>
+      <c r="I41" s="151"/>
       <c r="J41" s="9" t="s">
         <v>10</v>
       </c>
@@ -17015,17 +17015,17 @@
       <c r="B43" s="5">
         <v>1</v>
       </c>
-      <c r="C43" s="89" t="s">
+      <c r="C43" s="148" t="s">
         <v>231</v>
       </c>
-      <c r="D43" s="90"/>
-      <c r="E43" s="90"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="165" t="s">
+      <c r="D43" s="149"/>
+      <c r="E43" s="149"/>
+      <c r="F43" s="150"/>
+      <c r="G43" s="195" t="s">
         <v>230</v>
       </c>
-      <c r="H43" s="165"/>
-      <c r="I43" s="165"/>
+      <c r="H43" s="195"/>
+      <c r="I43" s="195"/>
       <c r="J43" s="5">
         <v>5</v>
       </c>
@@ -17038,13 +17038,13 @@
       <c r="B44" s="5">
         <v>2</v>
       </c>
-      <c r="C44" s="89"/>
-      <c r="D44" s="90"/>
-      <c r="E44" s="90"/>
-      <c r="F44" s="91"/>
-      <c r="G44" s="165"/>
-      <c r="H44" s="165"/>
-      <c r="I44" s="165"/>
+      <c r="C44" s="148"/>
+      <c r="D44" s="149"/>
+      <c r="E44" s="149"/>
+      <c r="F44" s="150"/>
+      <c r="G44" s="195"/>
+      <c r="H44" s="195"/>
+      <c r="I44" s="195"/>
       <c r="J44" s="5"/>
       <c r="K44" s="8" t="s">
         <v>118</v>
@@ -17055,13 +17055,13 @@
       <c r="B45" s="5">
         <v>3</v>
       </c>
-      <c r="C45" s="89"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="165"/>
-      <c r="H45" s="165"/>
-      <c r="I45" s="165"/>
+      <c r="C45" s="148"/>
+      <c r="D45" s="149"/>
+      <c r="E45" s="149"/>
+      <c r="F45" s="150"/>
+      <c r="G45" s="195"/>
+      <c r="H45" s="195"/>
+      <c r="I45" s="195"/>
       <c r="J45" s="5"/>
       <c r="K45" s="8" t="s">
         <v>118</v>
@@ -17072,13 +17072,13 @@
       <c r="B46" s="5">
         <v>4</v>
       </c>
-      <c r="C46" s="89"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="91"/>
-      <c r="G46" s="165"/>
-      <c r="H46" s="165"/>
-      <c r="I46" s="165"/>
+      <c r="C46" s="148"/>
+      <c r="D46" s="149"/>
+      <c r="E46" s="149"/>
+      <c r="F46" s="150"/>
+      <c r="G46" s="195"/>
+      <c r="H46" s="195"/>
+      <c r="I46" s="195"/>
       <c r="J46" s="5"/>
       <c r="K46" s="8" t="s">
         <v>118</v>
@@ -17089,13 +17089,13 @@
       <c r="B47" s="5">
         <v>5</v>
       </c>
-      <c r="C47" s="89"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="91"/>
-      <c r="G47" s="165"/>
-      <c r="H47" s="165"/>
-      <c r="I47" s="165"/>
+      <c r="C47" s="148"/>
+      <c r="D47" s="149"/>
+      <c r="E47" s="149"/>
+      <c r="F47" s="150"/>
+      <c r="G47" s="195"/>
+      <c r="H47" s="195"/>
+      <c r="I47" s="195"/>
       <c r="J47" s="5"/>
       <c r="K47" s="8" t="s">
         <v>118</v>
@@ -17106,13 +17106,13 @@
       <c r="B48" s="5">
         <v>6</v>
       </c>
-      <c r="C48" s="89"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="91"/>
-      <c r="G48" s="165"/>
-      <c r="H48" s="165"/>
-      <c r="I48" s="165"/>
+      <c r="C48" s="148"/>
+      <c r="D48" s="149"/>
+      <c r="E48" s="149"/>
+      <c r="F48" s="150"/>
+      <c r="G48" s="195"/>
+      <c r="H48" s="195"/>
+      <c r="I48" s="195"/>
       <c r="J48" s="5"/>
       <c r="K48" s="8" t="s">
         <v>118</v>
@@ -17123,13 +17123,13 @@
       <c r="B49" s="5">
         <v>7</v>
       </c>
-      <c r="C49" s="89"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="91"/>
-      <c r="G49" s="165"/>
-      <c r="H49" s="165"/>
-      <c r="I49" s="165"/>
+      <c r="C49" s="148"/>
+      <c r="D49" s="149"/>
+      <c r="E49" s="149"/>
+      <c r="F49" s="150"/>
+      <c r="G49" s="195"/>
+      <c r="H49" s="195"/>
+      <c r="I49" s="195"/>
       <c r="J49" s="5"/>
       <c r="K49" s="8" t="s">
         <v>118</v>
@@ -17140,13 +17140,13 @@
       <c r="B50" s="5">
         <v>8</v>
       </c>
-      <c r="C50" s="89"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="91"/>
-      <c r="G50" s="165"/>
-      <c r="H50" s="165"/>
-      <c r="I50" s="165"/>
+      <c r="C50" s="148"/>
+      <c r="D50" s="149"/>
+      <c r="E50" s="149"/>
+      <c r="F50" s="150"/>
+      <c r="G50" s="195"/>
+      <c r="H50" s="195"/>
+      <c r="I50" s="195"/>
       <c r="J50" s="6"/>
       <c r="K50" s="8" t="s">
         <v>118</v>
@@ -17157,13 +17157,13 @@
       <c r="B51" s="5">
         <v>9</v>
       </c>
-      <c r="C51" s="89"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="91"/>
-      <c r="G51" s="165"/>
-      <c r="H51" s="165"/>
-      <c r="I51" s="165"/>
+      <c r="C51" s="148"/>
+      <c r="D51" s="149"/>
+      <c r="E51" s="149"/>
+      <c r="F51" s="150"/>
+      <c r="G51" s="195"/>
+      <c r="H51" s="195"/>
+      <c r="I51" s="195"/>
       <c r="J51" s="6"/>
       <c r="K51" s="8" t="s">
         <v>118</v>
@@ -17174,13 +17174,13 @@
       <c r="B52" s="5">
         <v>10</v>
       </c>
-      <c r="C52" s="89"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="90"/>
-      <c r="F52" s="91"/>
-      <c r="G52" s="165"/>
-      <c r="H52" s="165"/>
-      <c r="I52" s="165"/>
+      <c r="C52" s="148"/>
+      <c r="D52" s="149"/>
+      <c r="E52" s="149"/>
+      <c r="F52" s="150"/>
+      <c r="G52" s="195"/>
+      <c r="H52" s="195"/>
+      <c r="I52" s="195"/>
       <c r="J52" s="6"/>
       <c r="K52" s="8" t="s">
         <v>118</v>
@@ -17189,84 +17189,84 @@
     </row>
     <row r="53" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="25"/>
-      <c r="C53" s="162"/>
-      <c r="D53" s="162"/>
-      <c r="E53" s="162"/>
-      <c r="F53" s="162"/>
-      <c r="G53" s="162"/>
-      <c r="H53" s="162"/>
-      <c r="I53" s="162"/>
+      <c r="C53" s="106"/>
+      <c r="D53" s="106"/>
+      <c r="E53" s="106"/>
+      <c r="F53" s="106"/>
+      <c r="G53" s="106"/>
+      <c r="H53" s="106"/>
+      <c r="I53" s="106"/>
       <c r="K53" s="7"/>
       <c r="L53" s="25"/>
     </row>
     <row r="54" spans="2:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="164" t="s">
+      <c r="B54" s="108" t="s">
         <v>120</v>
       </c>
-      <c r="C54" s="164"/>
-      <c r="D54" s="164"/>
-      <c r="E54" s="164"/>
-      <c r="F54" s="164"/>
-      <c r="G54" s="164"/>
-      <c r="H54" s="164"/>
-      <c r="I54" s="164"/>
-      <c r="J54" s="164"/>
-      <c r="K54" s="164"/>
-      <c r="L54" s="164"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="108"/>
+      <c r="F54" s="108"/>
+      <c r="G54" s="108"/>
+      <c r="H54" s="108"/>
+      <c r="I54" s="108"/>
+      <c r="J54" s="108"/>
+      <c r="K54" s="108"/>
+      <c r="L54" s="108"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="166" t="s">
+      <c r="B56" s="196" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="166"/>
-      <c r="D56" s="166"/>
-      <c r="E56" s="166"/>
-      <c r="F56" s="166"/>
-      <c r="G56" s="166"/>
-      <c r="H56" s="166"/>
-      <c r="I56" s="166"/>
-      <c r="J56" s="166"/>
-      <c r="K56" s="166"/>
-      <c r="L56" s="166"/>
+      <c r="C56" s="196"/>
+      <c r="D56" s="196"/>
+      <c r="E56" s="196"/>
+      <c r="F56" s="196"/>
+      <c r="G56" s="196"/>
+      <c r="H56" s="196"/>
+      <c r="I56" s="196"/>
+      <c r="J56" s="196"/>
+      <c r="K56" s="196"/>
+      <c r="L56" s="196"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="166"/>
-      <c r="C57" s="166"/>
-      <c r="D57" s="166"/>
-      <c r="E57" s="166"/>
-      <c r="F57" s="166"/>
-      <c r="G57" s="166"/>
-      <c r="H57" s="166"/>
-      <c r="I57" s="166"/>
-      <c r="J57" s="166"/>
-      <c r="K57" s="166"/>
-      <c r="L57" s="166"/>
+      <c r="B57" s="196"/>
+      <c r="C57" s="196"/>
+      <c r="D57" s="196"/>
+      <c r="E57" s="196"/>
+      <c r="F57" s="196"/>
+      <c r="G57" s="196"/>
+      <c r="H57" s="196"/>
+      <c r="I57" s="196"/>
+      <c r="J57" s="196"/>
+      <c r="K57" s="196"/>
+      <c r="L57" s="196"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="166"/>
-      <c r="C58" s="166"/>
-      <c r="D58" s="166"/>
-      <c r="E58" s="166"/>
-      <c r="F58" s="166"/>
-      <c r="G58" s="166"/>
-      <c r="H58" s="166"/>
-      <c r="I58" s="166"/>
-      <c r="J58" s="166"/>
-      <c r="K58" s="166"/>
-      <c r="L58" s="166"/>
+      <c r="B58" s="196"/>
+      <c r="C58" s="196"/>
+      <c r="D58" s="196"/>
+      <c r="E58" s="196"/>
+      <c r="F58" s="196"/>
+      <c r="G58" s="196"/>
+      <c r="H58" s="196"/>
+      <c r="I58" s="196"/>
+      <c r="J58" s="196"/>
+      <c r="K58" s="196"/>
+      <c r="L58" s="196"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="166"/>
-      <c r="C59" s="166"/>
-      <c r="D59" s="166"/>
-      <c r="E59" s="166"/>
-      <c r="F59" s="166"/>
-      <c r="G59" s="166"/>
-      <c r="H59" s="166"/>
-      <c r="I59" s="166"/>
-      <c r="J59" s="166"/>
-      <c r="K59" s="166"/>
-      <c r="L59" s="166"/>
+      <c r="B59" s="196"/>
+      <c r="C59" s="196"/>
+      <c r="D59" s="196"/>
+      <c r="E59" s="196"/>
+      <c r="F59" s="196"/>
+      <c r="G59" s="196"/>
+      <c r="H59" s="196"/>
+      <c r="I59" s="196"/>
+      <c r="J59" s="196"/>
+      <c r="K59" s="196"/>
+      <c r="L59" s="196"/>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
@@ -17278,55 +17278,26 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B6:L7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B1:L2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="B56:L59"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="B54:L54"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:I47"/>
     <mergeCell ref="C44:F44"/>
     <mergeCell ref="G44:I44"/>
     <mergeCell ref="I31:J31"/>
@@ -17343,26 +17314,55 @@
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="G43:I43"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="B56:L59"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="B54:L54"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B1:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B6:L7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>

</xml_diff>